<commit_message>
Generated schedule for 2025 Jan
</commit_message>
<xml_diff>
--- a/schedule_2024_12.xlsx
+++ b/schedule_2024_12.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ujjawal/Probe/doctor-sched/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0810F1-F4AC-1A44-89A2-0A72D8B686AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2463C3D-CA9C-0C44-927E-21E93DC86CA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="640" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -552,8 +552,8 @@
   <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="157" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G43" sqref="G43"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A42" sqref="A34:A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>